<commit_message>
Tweaking post crash levels
</commit_message>
<xml_diff>
--- a/Planning/chapter_1_sprint.xlsx
+++ b/Planning/chapter_1_sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Jeff\UnityProjects\journey\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D80A3-1E3D-403F-8994-792A485388EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883ED9B5-E147-4E7D-B4C4-625DBE004FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{01D23D36-369B-4BEE-9D83-54B753740F81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{01D23D36-369B-4BEE-9D83-54B753740F81}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,9 @@
     <sheet name="dialog tasks" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">bugs!$A$1:$D$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">bugs!$A$1:$D$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="84">
   <si>
     <t>background image</t>
   </si>
@@ -292,6 +291,9 @@
   </si>
   <si>
     <t>7 - release testing</t>
+  </si>
+  <si>
+    <t>picking up boxes stops working if you carry a box to a different level; also happens when you die during carry.</t>
   </si>
 </sst>
 </file>
@@ -350,7 +352,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +401,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -435,13 +443,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,16 +463,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6A92DC-2CE6-4761-9D01-469062FFD0DE}">
   <dimension ref="A1:BD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,76 +1281,76 @@
       <c r="A1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="17" t="s">
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="18" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="11" t="s">
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="11"/>
-      <c r="AQ1" s="18" t="s">
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="16" t="s">
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="19" t="s">
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="13"/>
+      <c r="BB1" s="13"/>
+      <c r="BC1" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1852,39 +1860,39 @@
       <c r="A5" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1892,72 +1900,72 @@
       <c r="A9" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="14"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="14"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="AP10" s="11" t="s">
+      <c r="AP10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AQ10" s="11"/>
+      <c r="AQ10" s="14"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
-      <c r="AR11" s="11" t="s">
+      <c r="AR11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AS11" s="11"/>
-      <c r="AT11" s="11"/>
-      <c r="AU11" s="11"/>
-      <c r="AV11" s="11"/>
-      <c r="AW11" s="11"/>
-      <c r="AX11" s="11"/>
-      <c r="AY11" s="11"/>
-      <c r="AZ11" s="11"/>
-      <c r="BA11" s="11"/>
+      <c r="AS11" s="14"/>
+      <c r="AT11" s="14"/>
+      <c r="AU11" s="14"/>
+      <c r="AV11" s="14"/>
+      <c r="AW11" s="14"/>
+      <c r="AX11" s="14"/>
+      <c r="AY11" s="14"/>
+      <c r="AZ11" s="14"/>
+      <c r="BA11" s="14"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
-      <c r="BB12" s="19" t="s">
+      <c r="BB12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="BC12" s="19"/>
+      <c r="BC12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1985,7 +1993,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,10 +2052,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088C03E8-59AF-44D1-862E-79A089A5A5D7}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,9 +2120,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>30</v>
@@ -2123,26 +2131,26 @@
         <v>34</v>
       </c>
       <c r="D5" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>33</v>
@@ -2156,7 +2164,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>33</v>
@@ -2165,13 +2173,27 @@
         <v>34</v>
       </c>
       <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D8" xr:uid="{5B428F76-2F32-4A26-8341-B2DE59C7D1C6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
-      <sortCondition ref="B1:B8"/>
+  <autoFilter ref="A1:D9" xr:uid="{5B428F76-2F32-4A26-8341-B2DE59C7D1C6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
+      <sortCondition ref="B1:B9"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2361,7 +2383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E564840-F180-4A7F-B5D1-6353AB9420BC}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>